<commit_message>
fix: final changes applied
</commit_message>
<xml_diff>
--- a/dist/Downloads Organizer Config.xlsx
+++ b/dist/Downloads Organizer Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JohanH\Documents\my-sandbox\downloads-organizer-v2\dist\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC9B77E8-E1AA-45F4-9E5F-6300374EE52C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44036882-694A-4E38-BEB1-473CA4E33BAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Config" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="46">
   <si>
     <t>Folder Name</t>
   </si>
@@ -34,6 +34,9 @@
     <t>png</t>
   </si>
   <si>
+    <t>jpeg</t>
+  </si>
+  <si>
     <t>jpg</t>
   </si>
   <si>
@@ -43,6 +46,12 @@
     <t>webp</t>
   </si>
   <si>
+    <t>ico</t>
+  </si>
+  <si>
+    <t>drawio</t>
+  </si>
+  <si>
     <t>PowerPoints</t>
   </si>
   <si>
@@ -52,6 +61,9 @@
     <t>ppt</t>
   </si>
   <si>
+    <t>Spreadsheets</t>
+  </si>
+  <si>
     <t>xlsx</t>
   </si>
   <si>
@@ -73,6 +85,18 @@
     <t>pdf</t>
   </si>
   <si>
+    <t>txt</t>
+  </si>
+  <si>
+    <t>md</t>
+  </si>
+  <si>
+    <t>html</t>
+  </si>
+  <si>
+    <t>Archive Files</t>
+  </si>
+  <si>
     <t>zip</t>
   </si>
   <si>
@@ -88,16 +112,19 @@
     <t>mp4</t>
   </si>
   <si>
+    <t>gif</t>
+  </si>
+  <si>
     <t>Music</t>
   </si>
   <si>
     <t>mp3</t>
   </si>
   <si>
-    <t>Fonts</t>
-  </si>
-  <si>
-    <t>ttf</t>
+    <t>LaTex</t>
+  </si>
+  <si>
+    <t>tex</t>
   </si>
   <si>
     <t>Executable</t>
@@ -106,58 +133,31 @@
     <t>exe</t>
   </si>
   <si>
-    <t>Spreadsheets</t>
-  </si>
-  <si>
-    <t>Archive Files</t>
-  </si>
-  <si>
-    <t>txt</t>
+    <t>msi</t>
   </si>
   <si>
     <t>Programming</t>
   </si>
   <si>
+    <t>py</t>
+  </si>
+  <si>
     <t>json</t>
   </si>
   <si>
-    <t>py</t>
-  </si>
-  <si>
-    <t>ico</t>
-  </si>
-  <si>
-    <t>jpeg</t>
-  </si>
-  <si>
-    <t>drawio</t>
-  </si>
-  <si>
-    <t>html</t>
+    <t>db</t>
+  </si>
+  <si>
+    <t>yml</t>
+  </si>
+  <si>
+    <t>yaml</t>
   </si>
   <si>
     <t>Outlook</t>
   </si>
   <si>
     <t>msg</t>
-  </si>
-  <si>
-    <t>LaTex</t>
-  </si>
-  <si>
-    <t>tex</t>
-  </si>
-  <si>
-    <t>db</t>
-  </si>
-  <si>
-    <t>msi</t>
-  </si>
-  <si>
-    <t>yml</t>
-  </si>
-  <si>
-    <t>yaml</t>
   </si>
 </sst>
 </file>
@@ -213,8 +213,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="ConfigTable" displayName="ConfigTable" ref="A1:B33">
-  <autoFilter ref="A1:B33" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="ConfigTable" displayName="ConfigTable" ref="A1:B34">
+  <autoFilter ref="A1:B34" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Folder Name"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Extension"/>
@@ -508,16 +508,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B33"/>
+  <dimension ref="A1:B34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
-    </sheetView>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="14.33203125" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -540,7 +535,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>35</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -548,7 +543,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -556,7 +551,7 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -564,7 +559,7 @@
         <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -572,7 +567,7 @@
         <v>2</v>
       </c>
       <c r="B7" t="s">
-        <v>34</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
@@ -580,199 +575,199 @@
         <v>2</v>
       </c>
       <c r="B8" t="s">
-        <v>36</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B9" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="B11" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="B12" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="B14" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="B15" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="B16" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="B17" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>37</v>
+        <v>22</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B20" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B21" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="B22" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="B23" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="B24" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="B25" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="B26" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="B27" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="B28" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="B29" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="B30" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="B31" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="B32" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
@@ -780,7 +775,15 @@
         <v>38</v>
       </c>
       <c r="B33" t="s">
-        <v>39</v>
+        <v>43</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>44</v>
+      </c>
+      <c r="B34" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>